<commit_message>
irgendwas im excel gemact?
irgendwas im excel gemact?
</commit_message>
<xml_diff>
--- a/data/aest_bildungsabschluss-kinder-eltern.xlsx
+++ b/data/aest_bildungsabschluss-kinder-eltern.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wu-my.sharepoint.com/personal/clara_himmelbauer_wu_ac_at/Documents/Dokumente/teaching/Inequality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wu-my.sharepoint.com/personal/clara_himmelbauer_wu_ac_at/Documents/Dokumente/teaching/Inequality/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{40614486-DCF1-4ECD-86F1-878310DE9D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{10338380-F01F-4903-93F8-F9685EF9B3AB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{10338380-F01F-4903-93F8-F9685EF9B3AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -217,10 +217,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="cells" xfId="3" xr:uid="{383ABD15-556F-484B-94CA-7C583826A523}"/>
@@ -2849,7 +2849,7 @@
   <dimension ref="A2:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,20 +2860,20 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
@@ -2930,29 +2930,29 @@
         <f>SUM(C7:F7)</f>
         <v>342668</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <f>C7/$G7</f>
         <v>0.22853607573511386</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <f t="shared" ref="I7:K7" si="0">D7/$G7</f>
         <v>0.39169691946723945</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>0.26936860167859267</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>0.11039840311905401</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <f>SUM(H7:K7)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -2972,29 +2972,29 @@
         <f t="shared" ref="G8:G18" si="1">SUM(C8:F8)</f>
         <v>379362</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <f t="shared" ref="H8:H18" si="2">C8/$G8</f>
         <v>9.0248891560040276E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <f t="shared" ref="I8:I18" si="3">D8/$G8</f>
         <v>0.38087894939398254</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <f t="shared" ref="J8:J18" si="4">E8/$G8</f>
         <v>0.34544313874346932</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <f t="shared" ref="K8:K18" si="5">F8/$G8</f>
         <v>0.18342902030250791</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <f t="shared" ref="L8:L18" si="6">SUM(H8:K8)</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -3014,29 +3014,29 @@
         <f t="shared" si="1"/>
         <v>409995</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <f t="shared" si="2"/>
         <v>6.3166623983219303E-2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <f t="shared" si="3"/>
         <v>0.21528067415456287</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <f t="shared" si="4"/>
         <v>0.38279491213307482</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <f t="shared" si="5"/>
         <v>0.33875778972914306</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -3056,29 +3056,29 @@
         <f t="shared" si="1"/>
         <v>152072</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <f t="shared" si="2"/>
         <v>4.4610447682676628E-2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <f t="shared" si="3"/>
         <v>7.3609869009416587E-2</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <f t="shared" si="4"/>
         <v>0.2920721763375243</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <f t="shared" si="5"/>
         <v>0.58970750697038243</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -3098,29 +3098,29 @@
         <f t="shared" si="1"/>
         <v>421853</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <f t="shared" si="2"/>
         <v>0.32434995128634858</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <f t="shared" si="3"/>
         <v>0.17504912848788559</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <f t="shared" si="4"/>
         <v>0.24181883262653103</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <f t="shared" si="5"/>
         <v>0.25878208759923482</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -3140,29 +3140,29 @@
         <f t="shared" si="1"/>
         <v>763284</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <f t="shared" si="2"/>
         <v>0.16613475456055676</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <f t="shared" si="3"/>
         <v>0.28728363230462056</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <f t="shared" si="4"/>
         <v>0.30061025778085221</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <f t="shared" si="5"/>
         <v>0.24597135535397047</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
@@ -3184,29 +3184,29 @@
         <f t="shared" si="1"/>
         <v>186991</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <f t="shared" si="2"/>
         <v>0.28389601638581535</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <f t="shared" si="3"/>
         <v>0.35266937980972346</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <f t="shared" si="4"/>
         <v>0.25556844981844046</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <f t="shared" si="5"/>
         <v>0.10786615398602072</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -3226,29 +3226,29 @@
         <f t="shared" si="1"/>
         <v>587059</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <f t="shared" si="2"/>
         <v>0.10444776419405886</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <f t="shared" si="3"/>
         <v>0.38455419301978166</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <f t="shared" si="4"/>
         <v>0.33613146208473083</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <f t="shared" si="5"/>
         <v>0.17486658070142866</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -3268,29 +3268,29 @@
         <f t="shared" si="1"/>
         <v>327050</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <f t="shared" si="2"/>
         <v>6.0700198746369054E-2</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="1">
         <f t="shared" si="3"/>
         <v>0.20594710288946644</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <f t="shared" si="4"/>
         <v>0.38898333588136369</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K15" s="1">
         <f t="shared" si="5"/>
         <v>0.34436936248280081</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -3310,29 +3310,29 @@
         <f t="shared" si="1"/>
         <v>153835</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <f t="shared" si="2"/>
         <v>4.6588877693632791E-2</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <f t="shared" si="3"/>
         <v>7.0016576201774622E-2</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <f t="shared" si="4"/>
         <v>0.28735333311665096</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <f t="shared" si="5"/>
         <v>0.59604121298794166</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>5</v>
       </c>
@@ -3352,29 +3352,29 @@
         <f t="shared" si="1"/>
         <v>451015</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <f t="shared" si="2"/>
         <v>0.31182333181823219</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <f t="shared" si="3"/>
         <v>0.18222897242885491</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <f t="shared" si="4"/>
         <v>0.2443022959325078</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <f t="shared" si="5"/>
         <v>0.26164539982040508</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>6</v>
       </c>
@@ -3394,220 +3394,220 @@
         <f t="shared" si="1"/>
         <v>763284</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <f t="shared" si="2"/>
         <v>0.16613475456055676</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <f t="shared" si="3"/>
         <v>0.28728363230462056</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <f t="shared" si="4"/>
         <v>0.30061025778085221</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="1">
         <f t="shared" si="5"/>
         <v>0.24597135535397047</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="1">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.22853607573511386</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>9.0248891560040276E-2</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>6.3166623983219303E-2</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>4.4610447682676628E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>0.39169691946723945</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>0.38087894939398254</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>0.21528067415456287</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>7.3609869009416587E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>0.26936860167859267</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>0.34544313874346932</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>0.38279491213307482</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>0.2920721763375243</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>0.11039840311905401</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>0.18342902030250791</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>0.33875778972914306</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>0.58970750697038243</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>0.28389601638581535</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>0.10444776419405886</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>6.0700198746369054E-2</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>4.6588877693632791E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>0.35266937980972346</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>0.38455419301978166</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>0.20594710288946644</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>7.0016576201774622E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>0.25556844981844046</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>0.33613146208473083</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>0.38898333588136369</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>0.28735333311665096</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>0.10786615398602072</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>0.17486658070142866</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>0.34436936248280081</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>0.59604121298794166</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>